<commit_message>
atualizei o meu use_case em excel
</commit_message>
<xml_diff>
--- a/use-cases/use-case-realizar-receita-ingredientes.xlsx
+++ b/use-cases/use-case-realizar-receita-ingredientes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Marques\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A2S\LI4\projeto-li4\use-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58A2D74-2601-40A0-B106-768DAB054D14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D862A63-94A6-4116-9CA8-B9BA02EAC85D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Actor input</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Realizar Receita (Ingredientes e SuperMercado)</t>
   </si>
   <si>
-    <t>Selecinar Receita</t>
-  </si>
-  <si>
     <t>Utilizador</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>4. Inicia a Receita</t>
   </si>
   <si>
-    <t>[Falta ingredientes]</t>
-  </si>
-  <si>
     <t>(passo 3)</t>
   </si>
   <si>
@@ -112,10 +106,16 @@
     <t>(passo 3.4)</t>
   </si>
   <si>
-    <t>3.4.1. Informa que não quer realizar Receita</t>
-  </si>
-  <si>
     <t>3.4.2. Cancela Realização de Receita</t>
+  </si>
+  <si>
+    <t>3.4.1. Informa que quer cancelar Receita</t>
+  </si>
+  <si>
+    <t>Estar Logado no Sistema</t>
+  </si>
+  <si>
+    <t>[Falta ingredientes] (passo 3)</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -351,6 +351,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,14 +378,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,16 +700,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
   <dimension ref="B1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="51.125" customWidth="1"/>
-    <col min="4" max="4" width="55.75" customWidth="1"/>
+    <col min="3" max="3" width="46.875" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -711,40 +717,40 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="11"/>
+      <c r="C3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="11"/>
+      <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="13"/>
+      <c r="C5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -755,120 +761,118 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="15"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="18"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="18"/>
+      <c r="C9" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
-        <v>23</v>
+      <c r="B11" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
-        <v>15</v>
+    <row r="12" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
+      <c r="D12" s="19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="B13" s="11"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="18"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="6"/>
       <c r="D15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="17" t="s">
-        <v>24</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="18" t="s">
-        <v>16</v>
+      <c r="B18" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
-        <v>24</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="18" t="s">
-        <v>27</v>
+      <c r="B21" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>

</xml_diff>

<commit_message>
o vpp do meu use case Realizar Receita Ingrediente
</commit_message>
<xml_diff>
--- a/use-cases/use-case-realizar-receita-ingredientes.xlsx
+++ b/use-cases/use-case-realizar-receita-ingredientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A2S\LI4\projeto-li4\use-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D862A63-94A6-4116-9CA8-B9BA02EAC85D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4259F67-2079-40D4-ADA5-81595A074A4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -152,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -161,6 +161,87 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -168,11 +249,26 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -183,16 +279,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -203,78 +292,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -287,47 +311,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -336,53 +321,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,7 +680,7 @@
   <dimension ref="B1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -744,52 +723,52 @@
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="18"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="18"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="18"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="18"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -798,37 +777,37 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="6"/>
       <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -837,7 +816,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="5"/>
@@ -846,14 +825,14 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -862,7 +841,7 @@
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="5"/>
@@ -871,7 +850,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="6"/>

</xml_diff>

<commit_message>
alterei os diagramas Selecionar Receita e Realizar Receita Ingredientes para ficar de acordo com o que o Petra disse
</commit_message>
<xml_diff>
--- a/use-cases/use-case-realizar-receita-ingredientes.xlsx
+++ b/use-cases/use-case-realizar-receita-ingredientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A2S\LI4\projeto-li4\use-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4259F67-2079-40D4-ADA5-81595A074A4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D60642-0F66-4E3D-9CF4-469FBE51882F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Actor input</t>
   </si>
@@ -58,36 +58,6 @@
     <t>Pronto para Iniciar Receita</t>
   </si>
   <si>
-    <t>1. «include» Selecionar Receita</t>
-  </si>
-  <si>
-    <t>2. Mostra Descrição da Receita e respetivos Ingredientes</t>
-  </si>
-  <si>
-    <t>3. Informa que quer Iniciar a Receita</t>
-  </si>
-  <si>
-    <t>4. Inicia a Receita</t>
-  </si>
-  <si>
-    <t>(passo 3)</t>
-  </si>
-  <si>
-    <t>3.1. Informa que faltam Ingredientes</t>
-  </si>
-  <si>
-    <t>3.2. Obtém localização Utilizador e calcula supermercados mais próximos</t>
-  </si>
-  <si>
-    <t>3.3. Mostra supermecados mais próximos</t>
-  </si>
-  <si>
-    <t>3.4. Informa que pode prosseguir com a Receita</t>
-  </si>
-  <si>
-    <t>3.5. Volta a 4.</t>
-  </si>
-  <si>
     <t>Cenário Excessão</t>
   </si>
   <si>
@@ -97,25 +67,52 @@
     <t>[Não quer Receita]</t>
   </si>
   <si>
-    <t>3.1. Informa que não quer realizar Receita</t>
-  </si>
-  <si>
-    <t>3.2. Cancela Realização de Receita</t>
-  </si>
-  <si>
-    <t>(passo 3.4)</t>
-  </si>
-  <si>
-    <t>3.4.2. Cancela Realização de Receita</t>
-  </si>
-  <si>
-    <t>3.4.1. Informa que quer cancelar Receita</t>
-  </si>
-  <si>
-    <t>Estar Logado no Sistema</t>
-  </si>
-  <si>
-    <t>[Falta ingredientes] (passo 3)</t>
+    <t>Ter Selecionado Receita</t>
+  </si>
+  <si>
+    <t>1. Mostra Descrição da Receita e respetivos Ingredientes</t>
+  </si>
+  <si>
+    <t>2. Informa que quer Iniciar a Receita</t>
+  </si>
+  <si>
+    <t>3. Inicia a Receita</t>
+  </si>
+  <si>
+    <t>[Falta ingredientes] (passo 2)</t>
+  </si>
+  <si>
+    <t>2.1. Informa que faltam Ingredientes</t>
+  </si>
+  <si>
+    <t>2.2. Obtém localização Utilizador e calcula supermercados mais próximos</t>
+  </si>
+  <si>
+    <t>2.5. Volta a 4.</t>
+  </si>
+  <si>
+    <t>2.4. Informa que pode prosseguir com a Receita</t>
+  </si>
+  <si>
+    <t>2.3. Mostra supermecados mais próximos</t>
+  </si>
+  <si>
+    <t>2.1. Informa que não quer realizar Receita</t>
+  </si>
+  <si>
+    <t>2.2. Cancela Realização de Receita</t>
+  </si>
+  <si>
+    <t>2.4.1. Informa que quer cancelar Receita</t>
+  </si>
+  <si>
+    <t>2.4.2. Cancela Realização de Receita</t>
+  </si>
+  <si>
+    <t>(passo 2.4)</t>
+  </si>
+  <si>
+    <t>(passo 2)</t>
   </si>
 </sst>
 </file>
@@ -345,6 +342,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -356,12 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D21"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -696,165 +693,158 @@
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="14"/>
+      <c r="C4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="16"/>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="11" t="s">
+    <row r="7" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="18"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="18"/>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="18"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="16"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="11" t="s">
-        <v>16</v>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="9"/>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="10"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="10"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="1" t="s">
+      <c r="B16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="3"/>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -862,7 +852,7 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
especificação do use case realizar receita ingredientes
</commit_message>
<xml_diff>
--- a/use-cases/use-case-realizar-receita-ingredientes.xlsx
+++ b/use-cases/use-case-realizar-receita-ingredientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A2S\LI4\projeto-li4\use-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D60642-0F66-4E3D-9CF4-469FBE51882F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FBE9D3-12EF-45E2-BCC9-EB56054F3084}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Actor input</t>
   </si>
@@ -49,70 +49,109 @@
     <t>Pós condição:</t>
   </si>
   <si>
-    <t>Realizar Receita (Ingredientes e SuperMercado)</t>
-  </si>
-  <si>
     <t>Utilizador</t>
   </si>
   <si>
     <t>Pronto para Iniciar Receita</t>
   </si>
   <si>
-    <t>Cenário Excessão</t>
-  </si>
-  <si>
-    <t>Cenário Alternativo</t>
-  </si>
-  <si>
     <t>[Não quer Receita]</t>
   </si>
   <si>
-    <t>Ter Selecionado Receita</t>
-  </si>
-  <si>
-    <t>1. Mostra Descrição da Receita e respetivos Ingredientes</t>
-  </si>
-  <si>
-    <t>2. Informa que quer Iniciar a Receita</t>
-  </si>
-  <si>
-    <t>3. Inicia a Receita</t>
-  </si>
-  <si>
-    <t>[Falta ingredientes] (passo 2)</t>
-  </si>
-  <si>
-    <t>2.1. Informa que faltam Ingredientes</t>
-  </si>
-  <si>
-    <t>2.2. Obtém localização Utilizador e calcula supermercados mais próximos</t>
-  </si>
-  <si>
-    <t>2.5. Volta a 4.</t>
-  </si>
-  <si>
-    <t>2.4. Informa que pode prosseguir com a Receita</t>
-  </si>
-  <si>
-    <t>2.3. Mostra supermecados mais próximos</t>
-  </si>
-  <si>
-    <t>2.1. Informa que não quer realizar Receita</t>
-  </si>
-  <si>
-    <t>2.2. Cancela Realização de Receita</t>
-  </si>
-  <si>
-    <t>2.4.1. Informa que quer cancelar Receita</t>
-  </si>
-  <si>
-    <t>2.4.2. Cancela Realização de Receita</t>
-  </si>
-  <si>
-    <t>(passo 2.4)</t>
-  </si>
-  <si>
-    <t>(passo 2)</t>
+    <t>Ter Pesquisado Receita</t>
+  </si>
+  <si>
+    <t>Selecionar Receita (Ingredientes e SuperMercado)</t>
+  </si>
+  <si>
+    <t>1. «include» Interpretar Comando de Voz</t>
+  </si>
+  <si>
+    <t>2. Mostra Descrição da Receita e respetivos Ingredientes</t>
+  </si>
+  <si>
+    <t>3. Informa que quer Iniciar a Receita</t>
+  </si>
+  <si>
+    <t>4. Inicia a Receita</t>
+  </si>
+  <si>
+    <t>3.1. Informa que faltam Ingredientes</t>
+  </si>
+  <si>
+    <t>3.4. Informa que pode prosseguir com a Receita</t>
+  </si>
+  <si>
+    <t>3.5. Volta a 4.</t>
+  </si>
+  <si>
+    <t>3.3. Mostra supermecados mais próximos</t>
+  </si>
+  <si>
+    <t>(passo 3)</t>
+  </si>
+  <si>
+    <t>3.2. Cancela Realização de Receita</t>
+  </si>
+  <si>
+    <t>3.1. Informa que não quer realizar Receita</t>
+  </si>
+  <si>
+    <t>3.4.1. Informa que quer cancelar Receita</t>
+  </si>
+  <si>
+    <t>3.4.2. Cancela Realização de Receita</t>
+  </si>
+  <si>
+    <t>(passo 3.4)</t>
+  </si>
+  <si>
+    <t>3.2. Obtém localização do Utilizador e calcula supermercados mais próximos</t>
+  </si>
+  <si>
+    <t>[Não tem GPS]</t>
+  </si>
+  <si>
+    <t>(passo 3.2)</t>
+  </si>
+  <si>
+    <t>3.2.1. Questiona o Utilizador qual a sua Localização</t>
+  </si>
+  <si>
+    <t>[Faltam ingredientes] (passo 3)</t>
+  </si>
+  <si>
+    <t>3.2.2. Fornece Localização</t>
+  </si>
+  <si>
+    <t>3.2.3. Volta a 3.3.</t>
+  </si>
+  <si>
+    <t>[Não fornece Localização]</t>
+  </si>
+  <si>
+    <t>(passo 3.2.2)</t>
+  </si>
+  <si>
+    <t>3.2.2.1. Informa que não quer fornecer Localização</t>
+  </si>
+  <si>
+    <t>3.2.2.2. Cancela Realização de Receita</t>
+  </si>
+  <si>
+    <t>Alternativa 1</t>
+  </si>
+  <si>
+    <t>Excessão 1</t>
+  </si>
+  <si>
+    <t>Excessão 2</t>
+  </si>
+  <si>
+    <t>Alternativa 2</t>
+  </si>
+  <si>
+    <t>Excessão 3</t>
   </si>
 </sst>
 </file>
@@ -674,18 +713,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D20"/>
+  <dimension ref="B1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="46.875" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="50.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -694,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="16"/>
     </row>
@@ -703,7 +742,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="16"/>
     </row>
@@ -712,7 +751,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" s="16"/>
     </row>
@@ -721,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="16"/>
     </row>
@@ -736,115 +775,174 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="18"/>
       <c r="C7" s="5"/>
       <c r="D7" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="18"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="18"/>
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="18"/>
-      <c r="C8" s="5" t="s">
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="18"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="18"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
+      <c r="D12" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="10"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="10"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3" t="s">
+    </row>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="10" t="s">
+    <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="3"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -852,7 +950,7 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B6:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>